<commit_message>
push some data files
</commit_message>
<xml_diff>
--- a/humanAndMouse/data/cross_validation_SVM_human_PSNP.xlsx
+++ b/humanAndMouse/data/cross_validation_SVM_human_PSNP.xlsx
@@ -67,13 +67,13 @@
     <t>tn</t>
   </si>
   <si>
-    <t>41</t>
+    <t>38</t>
   </si>
   <si>
     <t>正：1130.0负：1130.0</t>
   </si>
   <si>
-    <t>svmC:32.0gamma:4.0</t>
+    <t>svmC:14.2543794902gamma:4.0</t>
   </si>
 </sst>
 </file>
@@ -481,46 +481,46 @@
         <v>19</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9097345132743362</v>
+        <v>0.6920353982300885</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0.8442087814170319</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8194690265486726</v>
+        <v>0.476991150442478</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8194690265486726</v>
+        <v>0.476991150442478</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0.9070796460176991</v>
       </c>
       <c r="I2" t="n">
-        <v>0.904728906854473</v>
+        <v>0.6540357286002186</v>
       </c>
       <c r="J2" t="n">
-        <v>0.8997634622471449</v>
+        <v>0.6030891999362946</v>
       </c>
       <c r="K2" t="n">
-        <v>0.8997634622471449</v>
+        <v>0.6030891999362946</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8339950509996561</v>
+        <v>0.4286918432896029</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9135218106351319</v>
+        <v>0.7379716500900617</v>
       </c>
       <c r="N2" t="n">
-        <v>926</v>
+        <v>539</v>
       </c>
       <c r="O2" t="n">
-        <v>204</v>
+        <v>591</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="Q2" t="n">
-        <v>1130</v>
+        <v>1025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>